<commit_message>
chore: added test description to entry to test github action workflow
</commit_message>
<xml_diff>
--- a/pages/apps/uprn-service/config.xlsx
+++ b/pages/apps/uprn-service/config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NDSH\GitHub\UPRN-PoC\dev\UprnApp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NDSH\GitHub\dsh-content\dev\pages\apps\uprn-service\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A048425-B799-4B52-A555-88567A2954B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{056F7469-4E42-4018-B983-8D734329683D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="301" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5578" uniqueCount="2409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6039" uniqueCount="2438">
   <si>
     <t>DbId</t>
   </si>
@@ -7255,6 +7255,93 @@
   </si>
   <si>
     <t>https://nerc-digital-solutions-hub.github.io/dsh-metadata/UPRN/DEFRA/ModelledBackgroundPollution/info.json</t>
+  </si>
+  <si>
+    <t>Area is too large.</t>
+  </si>
+  <si>
+    <t>Aref is too larles_100e.</t>
+  </si>
+  <si>
+    <t>Arebbebe is too larles_50e.</t>
+  </si>
+  <si>
+    <t>Rreeb is too larles_20e.</t>
+  </si>
+  <si>
+    <t>Rref is too larles_10e.</t>
+  </si>
+  <si>
+    <t>Rredb is too larles_5e.</t>
+  </si>
+  <si>
+    <t>Rrebcdb is too larles_1e.</t>
+  </si>
+  <si>
+    <t>Aref is too larper_tier_local_authorities_dec_22_uk_boundaries_fullye.</t>
+  </si>
+  <si>
+    <t>Aree is too larunties_and_unitary_authorities_dec_23_uk_boundaries_fullye.</t>
+  </si>
+  <si>
+    <t>Rrecba is too larrds_dec_23_uk_boundaries_fullye.</t>
+  </si>
+  <si>
+    <t>Rreee is too larddle_layer_super_output_areas_dec_21_ew_boundaries_fully_clippede.</t>
+  </si>
+  <si>
+    <t>Rree is too larwer_layer_super_output_areas_dec_21_ew_boundaries_fully_clippede.</t>
+  </si>
+  <si>
+    <t>Ared is too larilt_up_areas_dec_22e.</t>
+  </si>
+  <si>
+    <t>Areacaf is too larrn_05e.</t>
+  </si>
+  <si>
+    <t>Rred is too larimatejust_grid_englande.</t>
+  </si>
+  <si>
+    <t>Rred is too larimatejust_lsoas_en_2011_2022_v3_2022e.</t>
+  </si>
+  <si>
+    <t>Rreba is too larimatejust_msoas_england_2011e.</t>
+  </si>
+  <si>
+    <t>Rrec is too larimatejust_grid_uke.</t>
+  </si>
+  <si>
+    <t>Rread is too larimatejust_lsoas_uk_2011_floode.</t>
+  </si>
+  <si>
+    <t>Rrefe is too larimatejust_lsoas_wa_2011_2022_v3_2022e.</t>
+  </si>
+  <si>
+    <t>Rrefc is too larght_time_average_noise_level_of_major_traffic_routes_and_populated_road_sources_11pm_to_7am_rounde.</t>
+  </si>
+  <si>
+    <t>Rreb is too larerage_24_hour_noise_level_of_major_traffic_routes_and_populated_road_sources_rounde.</t>
+  </si>
+  <si>
+    <t>Rref is too lary_time_average_noise_level_of_major_traffic_routes_and_populated_road_sources_7am_to_11pm_rounde.</t>
+  </si>
+  <si>
+    <t>Rrebb is too larght_time_average_noise_level_on_network_rail_and_hs1_routes_and_populated_rail_sources_11pm_to_7am_rounde.</t>
+  </si>
+  <si>
+    <t>Rrefade is too larerage_24_hour_noise_level_on_network_rail_and_hs1_routes_and_populated_rail_sources_rounde.</t>
+  </si>
+  <si>
+    <t>Rref is too lary_time_average_noise_level_on_network_rail_and_hs1_routes_and_populated_rail_sources_7am_to_11pm_rounde.</t>
+  </si>
+  <si>
+    <t>Rrefd is too larban_areas_required_to_undertake_strategic_noise_mapping_rounde.</t>
+  </si>
+  <si>
+    <t>Rreeff is too lardelled_background_pollution_rastere.</t>
+  </si>
+  <si>
+    <t>Rred is tannualannual r_air_mbp_benzene_annuale.</t>
   </si>
 </sst>
 </file>
@@ -8025,9 +8112,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:W65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L23" sqref="L23"/>
+      <selection pane="bottomLeft" activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8179,6 +8266,9 @@
       </c>
       <c r="T2" t="b">
         <v>0</v>
+      </c>
+      <c r="V2" t="s">
+        <v>2409</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
chore: config build test
</commit_message>
<xml_diff>
--- a/pages/apps/uprn-service/config.xlsx
+++ b/pages/apps/uprn-service/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NDSH\GitHub\dsh-content\dev\pages\apps\uprn-service\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{056F7469-4E42-4018-B983-8D734329683D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E3550BE-50C7-45C0-98AA-197EF1B3B083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="301" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6039" uniqueCount="2438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5580" uniqueCount="2410">
   <si>
     <t>DbId</t>
   </si>
@@ -7258,90 +7258,6 @@
   </si>
   <si>
     <t>Area is too large.</t>
-  </si>
-  <si>
-    <t>Aref is too larles_100e.</t>
-  </si>
-  <si>
-    <t>Arebbebe is too larles_50e.</t>
-  </si>
-  <si>
-    <t>Rreeb is too larles_20e.</t>
-  </si>
-  <si>
-    <t>Rref is too larles_10e.</t>
-  </si>
-  <si>
-    <t>Rredb is too larles_5e.</t>
-  </si>
-  <si>
-    <t>Rrebcdb is too larles_1e.</t>
-  </si>
-  <si>
-    <t>Aref is too larper_tier_local_authorities_dec_22_uk_boundaries_fullye.</t>
-  </si>
-  <si>
-    <t>Aree is too larunties_and_unitary_authorities_dec_23_uk_boundaries_fullye.</t>
-  </si>
-  <si>
-    <t>Rrecba is too larrds_dec_23_uk_boundaries_fullye.</t>
-  </si>
-  <si>
-    <t>Rreee is too larddle_layer_super_output_areas_dec_21_ew_boundaries_fully_clippede.</t>
-  </si>
-  <si>
-    <t>Rree is too larwer_layer_super_output_areas_dec_21_ew_boundaries_fully_clippede.</t>
-  </si>
-  <si>
-    <t>Ared is too larilt_up_areas_dec_22e.</t>
-  </si>
-  <si>
-    <t>Areacaf is too larrn_05e.</t>
-  </si>
-  <si>
-    <t>Rred is too larimatejust_grid_englande.</t>
-  </si>
-  <si>
-    <t>Rred is too larimatejust_lsoas_en_2011_2022_v3_2022e.</t>
-  </si>
-  <si>
-    <t>Rreba is too larimatejust_msoas_england_2011e.</t>
-  </si>
-  <si>
-    <t>Rrec is too larimatejust_grid_uke.</t>
-  </si>
-  <si>
-    <t>Rread is too larimatejust_lsoas_uk_2011_floode.</t>
-  </si>
-  <si>
-    <t>Rrefe is too larimatejust_lsoas_wa_2011_2022_v3_2022e.</t>
-  </si>
-  <si>
-    <t>Rrefc is too larght_time_average_noise_level_of_major_traffic_routes_and_populated_road_sources_11pm_to_7am_rounde.</t>
-  </si>
-  <si>
-    <t>Rreb is too larerage_24_hour_noise_level_of_major_traffic_routes_and_populated_road_sources_rounde.</t>
-  </si>
-  <si>
-    <t>Rref is too lary_time_average_noise_level_of_major_traffic_routes_and_populated_road_sources_7am_to_11pm_rounde.</t>
-  </si>
-  <si>
-    <t>Rrebb is too larght_time_average_noise_level_on_network_rail_and_hs1_routes_and_populated_rail_sources_11pm_to_7am_rounde.</t>
-  </si>
-  <si>
-    <t>Rrefade is too larerage_24_hour_noise_level_on_network_rail_and_hs1_routes_and_populated_rail_sources_rounde.</t>
-  </si>
-  <si>
-    <t>Rref is too lary_time_average_noise_level_on_network_rail_and_hs1_routes_and_populated_rail_sources_7am_to_11pm_rounde.</t>
-  </si>
-  <si>
-    <t>Rrefd is too larban_areas_required_to_undertake_strategic_noise_mapping_rounde.</t>
-  </si>
-  <si>
-    <t>Rreeff is too lardelled_background_pollution_rastere.</t>
-  </si>
-  <si>
-    <t>Rred is tannualannual r_air_mbp_benzene_annuale.</t>
   </si>
 </sst>
 </file>
@@ -8112,9 +8028,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:W65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V5" sqref="V5"/>
+      <selection pane="bottomLeft" activeCell="V3" sqref="V3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8322,6 +8238,9 @@
       </c>
       <c r="T3" t="b">
         <v>0</v>
+      </c>
+      <c r="V3" t="s">
+        <v>2409</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
chore: added description for reason tiles 50km is disabled
</commit_message>
<xml_diff>
--- a/pages/apps/uprn-service/config.xlsx
+++ b/pages/apps/uprn-service/config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29725"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NDSH\GitHub\dsh-content\dev\pages\apps\uprn-service\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CDA401B-1563-4DB6-9CB8-7D5EE0B21E28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A3C9B0D-B784-46BF-918B-FDC4B2F768EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="301" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5580" uniqueCount="2410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5581" uniqueCount="2410">
   <si>
     <t>DbId</t>
   </si>
@@ -7713,7 +7713,7 @@
   <dimension ref="A1:W65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L8" sqref="A1:L8"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8028,9 +8028,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:W65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G52" sqref="G52"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W4" sqref="W4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8294,6 +8294,9 @@
       </c>
       <c r="T4" t="b">
         <v>0</v>
+      </c>
+      <c r="V4" t="s">
+        <v>2404</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
chore: added air_temperature dataset json config in the uprn-service/config.xlsx
</commit_message>
<xml_diff>
--- a/pages/apps/uprn-service/config.xlsx
+++ b/pages/apps/uprn-service/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NDSH\GitHub\dsh-content\dev\pages\apps\uprn-service\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A3C9B0D-B784-46BF-918B-FDC4B2F768EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1586C45E-DEA8-4DBF-87D5-695904905001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="301" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="132" windowWidth="23040" windowHeight="12024" tabRatio="388" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="folders" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5581" uniqueCount="2410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5582" uniqueCount="2411">
   <si>
     <t>DbId</t>
   </si>
@@ -7258,6 +7258,9 @@
   </si>
   <si>
     <t>[modelled_background_pollution_raster_cells]</t>
+  </si>
+  <si>
+    <t>https://nerc-digital-solutions-hub.github.io/dsh-metadata/UPRN/MetOffice/AQREAN/Annual/SL/air_temperature/info.json</t>
   </si>
 </sst>
 </file>
@@ -8028,9 +8031,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:W65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W4" sqref="W4"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O50" sqref="O50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10475,6 +10478,9 @@
       <c r="M45">
         <v>7004</v>
       </c>
+      <c r="O45" s="3" t="s">
+        <v>2410</v>
+      </c>
       <c r="P45">
         <v>2</v>
       </c>
@@ -11620,6 +11626,7 @@
     <hyperlink ref="E65" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
     <hyperlink ref="O38" r:id="rId8" xr:uid="{71FF0051-ABE5-4973-9ED9-91F5EC5E19E7}"/>
     <hyperlink ref="O40" r:id="rId9" xr:uid="{356432AE-63BD-45AD-AFAA-748A8876906A}"/>
+    <hyperlink ref="O45" r:id="rId10" xr:uid="{4252AAA9-D643-4DFB-8757-57BF2C62AF79}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11629,9 +11636,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S2251"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1121" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1093" sqref="F1093"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1235" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1255" sqref="A1255"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11647,7 +11654,7 @@
     <col min="9" max="9" width="31.77734375" customWidth="1"/>
     <col min="10" max="10" width="98.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="126.88671875" customWidth="1"/>
     <col min="13" max="13" width="136.21875" customWidth="1"/>
     <col min="14" max="14" width="33.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="25.21875" customWidth="1"/>

</xml_diff>